<commit_message>
added pdf data.json report-checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esaotegroup-my.sharepoint.com/personal/marco_todde_esaote_com/Documents/INTEGRATION/FSE/accreditamento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esaotegroup.sharepoint.com/sites/EbitIT/INT/Progetti di Integrazione/IT - Italia/__FSE/Accreditamento/it-fse-accreditamento/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{0554E3F4-1FF1-41C4-99A0-467012434CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6927470F-0556-4950-B7F8-25CE15E1D8C1}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{0554E3F4-1FF1-41C4-99A0-467012434CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{626DB9E4-1532-4D2B-8A3A-E51AE8F2E803}"/>
   <bookViews>
-    <workbookView xWindow="58380" yWindow="-960" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1050" windowWidth="26250" windowHeight="14370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="141">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -687,6 +687,36 @@
   </si>
   <si>
     <t>subject_application_version: 2.1b34.x</t>
+  </si>
+  <si>
+    <t>5778b020f3522159</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.dc99d82c032f3b614725e1eeb1b868b4ef1dc22a6340a6187aeacc41e824920c.4200b408ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-08T16:18:24.143Z</t>
+  </si>
+  <si>
+    <t>l'applicativo non gestisce le conclusioni come campo separato dal testo del referto</t>
+  </si>
+  <si>
+    <t>2023-03-08T17:21:18.743Z</t>
+  </si>
+  <si>
+    <t>729f283b4adfc6d4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.187859189abe6ac7e64b26f66ea72529bab08fd6772df590fbf1422e7e57dc6e.e00595294b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.acd69857c2b944e280f2745e5db8eaa0cddd510501b35e875236f7f2ca46f6e7.df223dfdab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e78202ef5d70343b</t>
+  </si>
+  <si>
+    <t>2023-03-08T17:36:30.200Z</t>
   </si>
 </sst>
 </file>
@@ -2610,7 +2640,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2879,11 +2909,21 @@
       <c r="E10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
+      <c r="F10" s="17">
+        <v>44993</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
@@ -2913,12 +2953,24 @@
       <c r="E11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="F11" s="17">
+        <v>44993</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>134</v>
+      </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
@@ -2947,11 +2999,21 @@
       <c r="E12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
+      <c r="F12" s="17">
+        <v>44993</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>40</v>
+      </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -19796,12 +19858,30 @@
     <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
+    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
+    <ds:schemaRef ds:uri="74204614-352d-415a-b69e-46d10468735d"/>
+    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
A1#111EBITSRLXXXX valorizzazione ID nei tag Section
Aggiunta dei tag ID nelle section e aggionramento dei file RAD_VALIDAZIONE_TEST11.pdf, data.json e report-checklist.xlsx.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1DE15F-3254-4B1B-A229-80CA15471A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD470A8-2344-4998-9115-03C6B01F5035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="464" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -689,15 +689,6 @@
     <t>subject_application_version: 2.1b34.x</t>
   </si>
   <si>
-    <t>5778b020f3522159</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.dc99d82c032f3b614725e1eeb1b868b4ef1dc22a6340a6187aeacc41e824920c.4200b408ea^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-08T16:18:24.143Z</t>
-  </si>
-  <si>
     <t>l'applicativo non gestisce le conclusioni come campo separato dal testo del referto</t>
   </si>
   <si>
@@ -979,6 +970,15 @@
   </si>
   <si>
     <t>EBIT SRL</t>
+  </si>
+  <si>
+    <t>2023-04-06T18:28:31.133Z</t>
+  </si>
+  <si>
+    <t>2c9a3c70152daa99</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4593f5131573b1875ee37c7c650601063b1d344a6ddac47ca0324982cac35ab1.2b7b49a6c2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC6FE8D-20B5-4094-9F18-656AE8EE60BF}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2904,11 +2904,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T830"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="7"/>
@@ -3180,16 +3180,16 @@
         <v>30</v>
       </c>
       <c r="F10" s="17">
-        <v>44993</v>
+        <v>45022</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>133</v>
+        <v>225</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>131</v>
+        <v>226</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>40</v>
@@ -3227,19 +3227,19 @@
         <v>44993</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
@@ -3273,19 +3273,19 @@
         <v>44993</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -3319,13 +3319,13 @@
         <v>44994</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>40</v>
@@ -3363,37 +3363,37 @@
         <v>44994</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M14" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q14" s="19"/>
       <c r="R14" s="20"/>
       <c r="S14" s="35" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="T14" s="30" t="s">
         <v>125</v>
@@ -3419,37 +3419,37 @@
         <v>44994</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M15" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
       <c r="S15" s="35" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T15" s="30" t="s">
         <v>125</v>
@@ -3482,13 +3482,13 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20" t="s">
@@ -3519,37 +3519,37 @@
         <v>44994</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="19"/>
       <c r="L17" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M17" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O17" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="20"/>
       <c r="S17" s="35" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="T17" s="30" t="s">
         <v>125</v>
@@ -3575,29 +3575,29 @@
         <v>44994</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K18" s="19"/>
       <c r="L18" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M18" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P18" s="19" t="s">
         <v>100</v>
@@ -3605,7 +3605,7 @@
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
       <c r="S18" s="35" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="T18" s="30" t="s">
         <v>125</v>
@@ -3631,37 +3631,37 @@
         <v>44994</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K19" s="19"/>
       <c r="L19" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="20"/>
       <c r="S19" s="35" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T19" s="30" t="s">
         <v>125</v>
@@ -3687,37 +3687,37 @@
         <v>44995</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K20" s="19"/>
       <c r="L20" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O20" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
       <c r="S20" s="35" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="T20" s="30" t="s">
         <v>125</v>
@@ -3743,37 +3743,37 @@
         <v>44994</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K21" s="19"/>
       <c r="L21" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="O21" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
       <c r="S21" s="35" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="T21" s="30" t="s">
         <v>125</v>
@@ -3799,37 +3799,37 @@
         <v>44994</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K22" s="19"/>
       <c r="L22" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M22" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
       <c r="S22" s="35" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="T22" s="30" t="s">
         <v>125</v>
@@ -3855,37 +3855,37 @@
         <v>44994</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K23" s="19"/>
       <c r="L23" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M23" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
       <c r="S23" s="35" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T23" s="30" t="s">
         <v>125</v>
@@ -3911,29 +3911,29 @@
         <v>44995</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K24" s="19"/>
       <c r="L24" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M24" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P24" s="19" t="s">
         <v>100</v>
@@ -3941,7 +3941,7 @@
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
       <c r="S24" s="35" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T24" s="30" t="s">
         <v>125</v>
@@ -3967,37 +3967,37 @@
         <v>44994</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M25" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="O25" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
       <c r="S25" s="35" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="T25" s="30" t="s">
         <v>125</v>
@@ -4023,37 +4023,37 @@
         <v>44994</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K26" s="19"/>
       <c r="L26" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M26" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
       <c r="S26" s="35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="T26" s="30" t="s">
         <v>125</v>
@@ -4079,37 +4079,37 @@
         <v>44994</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K27" s="19"/>
       <c r="L27" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M27" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
       <c r="S27" s="35" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="T27" s="30" t="s">
         <v>125</v>
@@ -4139,7 +4139,7 @@
         <v>100</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
@@ -4173,37 +4173,37 @@
         <v>44995</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K29" s="19"/>
       <c r="L29" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M29" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="O29" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q29" s="19"/>
       <c r="R29" s="20"/>
       <c r="S29" s="35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="T29" s="30" t="s">
         <v>125</v>
@@ -4233,7 +4233,7 @@
         <v>100</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -4271,7 +4271,7 @@
         <v>100</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
@@ -4309,7 +4309,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -4347,7 +4347,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
@@ -4385,7 +4385,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
@@ -4419,37 +4419,37 @@
         <v>44995</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K35" s="19"/>
       <c r="L35" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="M35" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="O35" s="19" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="P35" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="20"/>
       <c r="S35" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="T35" s="30" t="s">
         <v>125</v>
@@ -20223,15 +20223,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -20481,6 +20472,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -20501,14 +20501,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20528,6 +20520,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
A1#111EBITSRLXXXX aggiornamento test case
aggiornati i test case 11 e 12 con ID Section e campi opzionali come richiesto via mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD470A8-2344-4998-9115-03C6B01F5035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180C0042-99F1-4825-A3AB-7C5C0048415C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="464" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="227">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -689,18 +689,6 @@
     <t>subject_application_version: 2.1b34.x</t>
   </si>
   <si>
-    <t>l'applicativo non gestisce le conclusioni come campo separato dal testo del referto</t>
-  </si>
-  <si>
-    <t>2023-03-08T17:21:18.743Z</t>
-  </si>
-  <si>
-    <t>729f283b4adfc6d4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.187859189abe6ac7e64b26f66ea72529bab08fd6772df590fbf1422e7e57dc6e.e00595294b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.acd69857c2b944e280f2745e5db8eaa0cddd510501b35e875236f7f2ca46f6e7.df223dfdab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
@@ -979,6 +967,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.4593f5131573b1875ee37c7c650601063b1d344a6ddac47ca0324982cac35ab1.2b7b49a6c2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-07T09:31:51.547Z</t>
+  </si>
+  <si>
+    <t>a7329aa9dd6894c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.b6e9cc7d6e35348960a1e69139949d231d3400619b002067638abc31c5b4242e.4e6c1f288f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2908,7 +2905,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2953,7 +2950,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="7"/>
@@ -3183,13 +3180,13 @@
         <v>45022</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>40</v>
@@ -3224,23 +3221,21 @@
         <v>32</v>
       </c>
       <c r="F11" s="17">
-        <v>44993</v>
+        <v>45023</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>133</v>
+        <v>225</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>134</v>
+        <v>226</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="K11" s="19"/>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
@@ -3273,19 +3268,19 @@
         <v>44993</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J12" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -3319,13 +3314,13 @@
         <v>44994</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>40</v>
@@ -3363,13 +3358,13 @@
         <v>44994</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>40</v>
@@ -3382,18 +3377,18 @@
         <v>100</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="O14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q14" s="19"/>
       <c r="R14" s="20"/>
       <c r="S14" s="35" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="T14" s="30" t="s">
         <v>125</v>
@@ -3419,13 +3414,13 @@
         <v>44994</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>40</v>
@@ -3438,18 +3433,18 @@
         <v>100</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
       <c r="S15" s="35" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="T15" s="30" t="s">
         <v>125</v>
@@ -3482,13 +3477,13 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20" t="s">
@@ -3519,13 +3514,13 @@
         <v>44994</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J17" s="19" t="s">
         <v>40</v>
@@ -3538,18 +3533,18 @@
         <v>100</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="O17" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q17" s="19"/>
       <c r="R17" s="20"/>
       <c r="S17" s="35" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="T17" s="30" t="s">
         <v>125</v>
@@ -3575,13 +3570,13 @@
         <v>44994</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>40</v>
@@ -3594,7 +3589,7 @@
         <v>100</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>40</v>
@@ -3605,7 +3600,7 @@
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
       <c r="S18" s="35" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="T18" s="30" t="s">
         <v>125</v>
@@ -3631,13 +3626,13 @@
         <v>44994</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>40</v>
@@ -3650,18 +3645,18 @@
         <v>100</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="O19" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="20"/>
       <c r="S19" s="35" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="T19" s="30" t="s">
         <v>125</v>
@@ -3687,13 +3682,13 @@
         <v>44995</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>40</v>
@@ -3706,18 +3701,18 @@
         <v>100</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
       <c r="S20" s="35" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="T20" s="30" t="s">
         <v>125</v>
@@ -3743,13 +3738,13 @@
         <v>44994</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>40</v>
@@ -3762,18 +3757,18 @@
         <v>100</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
       <c r="S21" s="35" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="T21" s="30" t="s">
         <v>125</v>
@@ -3799,13 +3794,13 @@
         <v>44994</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>40</v>
@@ -3818,18 +3813,18 @@
         <v>100</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="O22" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
       <c r="S22" s="35" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="T22" s="30" t="s">
         <v>125</v>
@@ -3855,13 +3850,13 @@
         <v>44994</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>40</v>
@@ -3874,18 +3869,18 @@
         <v>100</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
       <c r="S23" s="35" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="T23" s="30" t="s">
         <v>125</v>
@@ -3911,13 +3906,13 @@
         <v>44995</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>40</v>
@@ -3930,7 +3925,7 @@
         <v>100</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>40</v>
@@ -3941,7 +3936,7 @@
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
       <c r="S24" s="35" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="T24" s="30" t="s">
         <v>125</v>
@@ -3967,13 +3962,13 @@
         <v>44994</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>40</v>
@@ -3986,18 +3981,18 @@
         <v>100</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
       <c r="S25" s="35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="T25" s="30" t="s">
         <v>125</v>
@@ -4023,13 +4018,13 @@
         <v>44994</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>40</v>
@@ -4042,18 +4037,18 @@
         <v>100</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
       <c r="S26" s="35" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="T26" s="30" t="s">
         <v>125</v>
@@ -4079,13 +4074,13 @@
         <v>44994</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>40</v>
@@ -4098,18 +4093,18 @@
         <v>100</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
       <c r="S27" s="35" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="T27" s="30" t="s">
         <v>125</v>
@@ -4139,7 +4134,7 @@
         <v>100</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
@@ -4173,13 +4168,13 @@
         <v>44995</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>40</v>
@@ -4192,18 +4187,18 @@
         <v>100</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="O29" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q29" s="19"/>
       <c r="R29" s="20"/>
       <c r="S29" s="35" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="T29" s="30" t="s">
         <v>125</v>
@@ -4233,7 +4228,7 @@
         <v>100</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -4271,7 +4266,7 @@
         <v>100</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
@@ -4309,7 +4304,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -4347,7 +4342,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
@@ -4385,7 +4380,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
@@ -4419,13 +4414,13 @@
         <v>44995</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>40</v>
@@ -4438,18 +4433,18 @@
         <v>100</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O35" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P35" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="20"/>
       <c r="S35" s="35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="T35" s="30" t="s">
         <v>125</v>
@@ -20223,6 +20218,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -20472,15 +20476,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -20501,6 +20496,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20520,14 +20523,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
A1#111EBITSRLXXXX Corretta gestione errori in report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180C0042-99F1-4825-A3AB-7C5C0048415C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144E69F4-8AA4-44E2-A7B2-BC4628837EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="464" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31005" yWindow="90" windowWidth="24855" windowHeight="15555" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="210">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -689,27 +689,6 @@
     <t>subject_application_version: 2.1b34.x</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.acd69857c2b944e280f2745e5db8eaa0cddd510501b35e875236f7f2ca46f6e7.df223dfdab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>e78202ef5d70343b</t>
-  </si>
-  <si>
-    <t>2023-03-08T17:36:30.200Z</t>
-  </si>
-  <si>
-    <t>c049c710b19711c7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.39e5f3ab703f95bbef517b6ec82973d0e6e2cb349d7ae5f2196fcb2bbcec4f4f.c28f8357be^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-09T10:10:47.263Z</t>
-  </si>
-  <si>
-    <t>storia clinica e suggerimenti per il medico non sono campi gestiti dall'applicativo</t>
-  </si>
-  <si>
     <t>948da432939ef3c4</t>
   </si>
   <si>
@@ -731,30 +710,6 @@
     <t>title : "Campo token JWT non valido.", "detail" : "Il campo action_id non Ã¨ corretto"</t>
   </si>
   <si>
-    <t>per eseguireil test è stato forzato a mano il campo action id a TEST</t>
-  </si>
-  <si>
-    <t>4814701ee9ca56b3</t>
-  </si>
-  <si>
-    <t>"title" : "Campo token JWT non valido.", "detail" : "Il campo person_id non Ã¨ valorizzato", "instance" : "/jwt-mandatory-field-missing"</t>
-  </si>
-  <si>
-    <t>l'applicativo non consente l'invio senza la presenza del Codice Fiscale, per i test è stato forzato vuoto e bypassati i sistemi di validazione interni.</t>
-  </si>
-  <si>
-    <t>2023-03-09T13:15:16.300Z</t>
-  </si>
-  <si>
-    <t>2023-03-09T14:52:20.840Z</t>
-  </si>
-  <si>
-    <t>aa4bfb227bc23ebe</t>
-  </si>
-  <si>
-    <t>"title" : "Campo token JWT non valido.", "detail" : "Il codice fiscale nel campo person_id non Ã¨ corretto", "instance" : "/jwt-mandatory-field-malformed"</t>
-  </si>
-  <si>
     <t>l'applicativo consente i vaori N e V, è stato forzato per il test il valore R</t>
   </si>
   <si>
@@ -896,18 +851,6 @@
     <t>52fd375a8c189cb0</t>
   </si>
   <si>
-    <t>2023-03-10T13:07:46.997Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.287f835b5e7251d5c219cdf94b1d479d291c97afcb0986fe5c9ac7768dd3e476.2f453a8ba4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>64607fd7aac52204</t>
-  </si>
-  <si>
-    <t>l'applicativo non consente di lasciar vuota la città di residenza, abbiamo svuotato a mano il campo per eseguire il test.</t>
-  </si>
-  <si>
     <t>[ERRORE-39| inFulfillmentOf/order/priorityCode DEVE avere l'attributo '@codeSystem='2.16.840.1.113883.5.7' e @code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM' ]</t>
   </si>
   <si>
@@ -935,12 +878,6 @@
     <t>2023-03-10T13:59:50.070Z</t>
   </si>
   <si>
-    <t>per eseguireil test è stato forzato a mano il campo purpose of use vuoto</t>
-  </si>
-  <si>
-    <t>l'applicativo converte in maiuscoli eventuali caratteri minuscoli, per il test abbiamo forzato il valore</t>
-  </si>
-  <si>
     <t>il valore del priorityCode è stato forzato con un valore non consentito per poter eseguire il test</t>
   </si>
   <si>
@@ -950,13 +887,6 @@
     <t>non verificabile</t>
   </si>
   <si>
-    <t>non verifcabile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"[ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'.  
-</t>
-  </si>
-  <si>
     <t>EBIT SRL</t>
   </si>
   <si>
@@ -976,6 +906,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.b6e9cc7d6e35348960a1e69139949d231d3400619b002067638abc31c5b4242e.4e6c1f288f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>i campi opzionali storia clinica e suggerimenti per il medico non sono campi gestiti dall'applicativo</t>
+  </si>
+  <si>
+    <t>le sezioni opzionali del test case non sono gestite</t>
+  </si>
+  <si>
+    <t>il campo è obbligatorio nell'applicativo</t>
+  </si>
+  <si>
+    <t>l'applicativo converte in maiuscoli eventuali caratteri minuscoli, non ammessi</t>
+  </si>
+  <si>
+    <t>l'indirizzo di residenza non è gestito perché opzionale</t>
+  </si>
+  <si>
+    <t>segnalato nella maschera di monitoraggio integrazioni</t>
   </si>
 </sst>
 </file>
@@ -2902,10 +2850,10 @@
   <dimension ref="A1:T830"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,7 +2898,7 @@
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="41" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="D2" s="40"/>
       <c r="F2" s="7"/>
@@ -3180,13 +3128,13 @@
         <v>45022</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="J10" s="19" t="s">
         <v>40</v>
@@ -3224,13 +3172,13 @@
         <v>45023</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="J11" s="19" t="s">
         <v>40</v>
@@ -3264,23 +3212,15 @@
       <c r="E12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="17">
-        <v>44993</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>131</v>
-      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
       <c r="J12" s="19" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
@@ -3310,22 +3250,16 @@
       <c r="E13" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>135</v>
-      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="19"/>
+        <v>100</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
@@ -3358,38 +3292,36 @@
         <v>44994</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="J14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K14" s="19"/>
       <c r="L14" s="19" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="M14" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="O14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="Q14" s="19"/>
       <c r="R14" s="20"/>
-      <c r="S14" s="35" t="s">
-        <v>213</v>
-      </c>
+      <c r="S14" s="35"/>
       <c r="T14" s="30" t="s">
         <v>125</v>
       </c>
@@ -3414,38 +3346,36 @@
         <v>44994</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="19" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="M15" s="19" t="s">
         <v>100</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="Q15" s="19"/>
       <c r="R15" s="20"/>
-      <c r="S15" s="35" t="s">
-        <v>145</v>
-      </c>
+      <c r="S15" s="35"/>
       <c r="T15" s="30" t="s">
         <v>125</v>
       </c>
@@ -3477,13 +3407,13 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="Q16" s="19"/>
       <c r="R16" s="20" t="s">
@@ -3510,42 +3440,24 @@
       <c r="E17" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>140</v>
-      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
       <c r="J17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="N17" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="O17" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="19" t="s">
-        <v>217</v>
-      </c>
+      <c r="K17" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="20"/>
-      <c r="S17" s="35" t="s">
-        <v>148</v>
-      </c>
+      <c r="S17" s="35"/>
       <c r="T17" s="30" t="s">
         <v>125</v>
       </c>
@@ -3566,42 +3478,24 @@
       <c r="E18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="I18" s="18" t="s">
-        <v>140</v>
-      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M18" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="O18" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P18" s="19" t="s">
-        <v>100</v>
-      </c>
+      <c r="K18" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
       <c r="R18" s="20"/>
-      <c r="S18" s="35" t="s">
-        <v>214</v>
-      </c>
+      <c r="S18" s="35"/>
       <c r="T18" s="30" t="s">
         <v>125</v>
       </c>
@@ -3626,13 +3520,13 @@
         <v>44994</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>40</v>
@@ -3645,18 +3539,18 @@
         <v>100</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="O19" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q19" s="19"/>
       <c r="R19" s="20"/>
       <c r="S19" s="35" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="T19" s="30" t="s">
         <v>125</v>
@@ -3678,42 +3572,24 @@
       <c r="E20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>201</v>
-      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
       <c r="J20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="N20" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="O20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>218</v>
-      </c>
+      <c r="K20" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
       <c r="R20" s="20"/>
-      <c r="S20" s="35" t="s">
-        <v>203</v>
-      </c>
+      <c r="S20" s="35"/>
       <c r="T20" s="30" t="s">
         <v>125</v>
       </c>
@@ -3738,13 +3614,13 @@
         <v>44994</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>40</v>
@@ -3757,18 +3633,18 @@
         <v>100</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="O21" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
       <c r="S21" s="35" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="T21" s="30" t="s">
         <v>125</v>
@@ -3794,13 +3670,13 @@
         <v>44994</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>40</v>
@@ -3813,18 +3689,18 @@
         <v>100</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="O22" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
       <c r="S22" s="35" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="T22" s="30" t="s">
         <v>125</v>
@@ -3850,13 +3726,13 @@
         <v>44994</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>40</v>
@@ -3869,18 +3745,18 @@
         <v>100</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
       <c r="S23" s="35" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="T23" s="30" t="s">
         <v>125</v>
@@ -3906,13 +3782,13 @@
         <v>44995</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>40</v>
@@ -3925,7 +3801,7 @@
         <v>100</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="O24" s="19" t="s">
         <v>40</v>
@@ -3936,7 +3812,7 @@
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
       <c r="S24" s="35" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="T24" s="30" t="s">
         <v>125</v>
@@ -3962,13 +3838,13 @@
         <v>44994</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>40</v>
@@ -3981,18 +3857,18 @@
         <v>100</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P25" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
       <c r="S25" s="35" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="T25" s="30" t="s">
         <v>125</v>
@@ -4018,13 +3894,13 @@
         <v>44994</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>40</v>
@@ -4037,18 +3913,18 @@
         <v>100</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P26" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
       <c r="S26" s="35" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="T26" s="30" t="s">
         <v>125</v>
@@ -4074,13 +3950,13 @@
         <v>44994</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>40</v>
@@ -4093,18 +3969,18 @@
         <v>100</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P27" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
       <c r="S27" s="35" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="T27" s="30" t="s">
         <v>125</v>
@@ -4134,7 +4010,7 @@
         <v>100</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
@@ -4168,13 +4044,13 @@
         <v>44995</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>40</v>
@@ -4187,18 +4063,18 @@
         <v>100</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="O29" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P29" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q29" s="19"/>
       <c r="R29" s="20"/>
       <c r="S29" s="35" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="T29" s="30" t="s">
         <v>125</v>
@@ -4228,7 +4104,7 @@
         <v>100</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -4266,7 +4142,7 @@
         <v>100</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
@@ -4304,7 +4180,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -4342,7 +4218,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
@@ -4380,7 +4256,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
@@ -4414,13 +4290,13 @@
         <v>44995</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="H35" s="18" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>40</v>
@@ -4433,18 +4309,18 @@
         <v>100</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="O35" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P35" s="19" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="Q35" s="19"/>
       <c r="R35" s="20"/>
       <c r="S35" s="35" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="T35" s="30" t="s">
         <v>125</v>
@@ -20218,15 +20094,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -20476,6 +20343,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
@@ -20496,14 +20372,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20523,6 +20391,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
EBITSRL upload files per accreditamento LDO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D6CE58-1D12-4D06-96B9-AA6D18876E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E088FC-F6DE-43E8-889E-363C3FBED9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="17520" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="28875" windowHeight="15480" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="218">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -927,12 +927,68 @@
 Nelle evidenze dell’errore viene anche registrato  l'errore ricevuto:
 "title" : "Errore semantico.", "detail" : "[ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR' ]</t>
   </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-09-20T15:42:36.960Z</t>
+  </si>
+  <si>
+    <t>ba744235c0982da3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a8a52ff8607a2e5ed11b83cb04d452bf3a9ed38d6e681f109347757dd84edfd9.0061e771fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>l'ospedalizzazione legata alla BPCO non viene trattata poiché Suitestensa è utilizzato per le lettere di dimissione in ambito cardiologico</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t>2023-09-20T17:23:39.103Z</t>
+  </si>
+  <si>
+    <t>0cb7f69dd5903495</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.f57eaf84fca19f8a37acfbc97d9312c3131f1f1e6c7bdb0fd3955da4cb4bfaa7.3417077500^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
+Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1033,6 +1089,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1284,7 +1345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1405,6 +1466,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2849,13 +2937,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T830"/>
+  <dimension ref="A1:T834"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,173 +3198,169 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+    <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49">
+        <v>6</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>203</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>204</v>
+      </c>
+      <c r="F10" s="52">
+        <v>45189</v>
+      </c>
+      <c r="G10" s="53" t="s">
+        <v>205</v>
+      </c>
+      <c r="H10" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="I10" s="53" t="s">
+        <v>207</v>
+      </c>
+      <c r="J10" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="56"/>
+      <c r="T10" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49">
+        <v>7</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>208</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54" t="s">
+        <v>100</v>
+      </c>
+      <c r="K11" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49">
+        <v>8</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" s="52">
+        <v>45189</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="54"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49">
+        <v>9</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="52"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="54"/>
+      <c r="O13" s="54"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
         <v>11</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="17">
-        <v>45022</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>12</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="17">
-        <v>45023</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>13</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
-        <v>14</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
-        <v>31</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>25</v>
@@ -3285,21 +3369,27 @@
         <v>28</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+        <v>29</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="17">
+        <v>45022</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="J14" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>191</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
@@ -3309,12 +3399,12 @@
       <c r="R14" s="20"/>
       <c r="S14" s="35"/>
       <c r="T14" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>25</v>
@@ -3323,21 +3413,27 @@
         <v>28</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+        <v>31</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="17">
+        <v>45023</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>185</v>
+      </c>
       <c r="J15" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>191</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
@@ -3347,12 +3443,12 @@
       <c r="R15" s="20"/>
       <c r="S15" s="35"/>
       <c r="T15" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>25</v>
@@ -3361,42 +3457,36 @@
         <v>28</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K16" s="19"/>
+        <v>100</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>186</v>
+      </c>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
-      <c r="N16" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="O16" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>178</v>
-      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
-      <c r="R16" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="R16" s="20"/>
       <c r="S16" s="35"/>
       <c r="T16" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>25</v>
@@ -3405,10 +3495,10 @@
         <v>28</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
@@ -3418,7 +3508,7 @@
         <v>100</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
@@ -3429,12 +3519,12 @@
       <c r="R17" s="20"/>
       <c r="S17" s="35"/>
       <c r="T17" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>25</v>
@@ -3443,10 +3533,10 @@
         <v>28</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>48</v>
+        <v>41</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>126</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="18"/>
@@ -3456,7 +3546,7 @@
         <v>100</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
@@ -3470,9 +3560,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>25</v>
@@ -3481,54 +3571,36 @@
         <v>28</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>144</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M19" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N19" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="O19" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P19" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
       <c r="R19" s="20"/>
-      <c r="S19" s="35" t="s">
-        <v>131</v>
-      </c>
+      <c r="S19" s="35"/>
       <c r="T19" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>25</v>
@@ -3537,36 +3609,42 @@
         <v>28</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>190</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="K20" s="19"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
+      <c r="N20" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="O20" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>178</v>
+      </c>
       <c r="Q20" s="19"/>
-      <c r="R20" s="20"/>
+      <c r="R20" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="S20" s="35"/>
       <c r="T20" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>25</v>
@@ -3575,54 +3653,36 @@
         <v>28</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>142</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
       <c r="J21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N21" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="O21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P21" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="20"/>
-      <c r="S21" s="35" t="s">
-        <v>132</v>
-      </c>
+      <c r="S21" s="35"/>
       <c r="T21" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>25</v>
@@ -3631,54 +3691,36 @@
         <v>28</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>139</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
       <c r="J22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N22" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="O22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P22" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="20"/>
-      <c r="S22" s="35" t="s">
-        <v>133</v>
-      </c>
+      <c r="S22" s="35"/>
       <c r="T22" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>25</v>
@@ -3687,22 +3729,22 @@
         <v>28</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F23" s="17">
         <v>44994</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>40</v>
@@ -3715,7 +3757,7 @@
         <v>40</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>40</v>
@@ -3726,15 +3768,15 @@
       <c r="Q23" s="19"/>
       <c r="R23" s="20"/>
       <c r="S23" s="35" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="T23" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>25</v>
@@ -3743,54 +3785,36 @@
         <v>28</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>170</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
       <c r="J24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="O24" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P24" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="20"/>
-      <c r="S24" s="35" t="s">
-        <v>177</v>
-      </c>
+      <c r="S24" s="35"/>
       <c r="T24" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>25</v>
@@ -3799,22 +3823,22 @@
         <v>28</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F25" s="17">
         <v>44994</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>40</v>
@@ -3827,7 +3851,7 @@
         <v>40</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O25" s="19" t="s">
         <v>40</v>
@@ -3838,7 +3862,7 @@
       <c r="Q25" s="19"/>
       <c r="R25" s="20"/>
       <c r="S25" s="35" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="T25" s="30" t="s">
         <v>125</v>
@@ -3846,7 +3870,7 @@
     </row>
     <row r="26" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>25</v>
@@ -3855,22 +3879,22 @@
         <v>28</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F26" s="17">
         <v>44994</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>40</v>
@@ -3883,7 +3907,7 @@
         <v>40</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O26" s="19" t="s">
         <v>40</v>
@@ -3894,7 +3918,7 @@
       <c r="Q26" s="19"/>
       <c r="R26" s="20"/>
       <c r="S26" s="35" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="T26" s="30" t="s">
         <v>125</v>
@@ -3902,7 +3926,7 @@
     </row>
     <row r="27" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>25</v>
@@ -3911,22 +3935,22 @@
         <v>28</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F27" s="17">
         <v>44994</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>40</v>
@@ -3939,7 +3963,7 @@
         <v>40</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O27" s="19" t="s">
         <v>40</v>
@@ -3950,15 +3974,15 @@
       <c r="Q27" s="19"/>
       <c r="R27" s="20"/>
       <c r="S27" s="35" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="T27" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>25</v>
@@ -3967,36 +3991,54 @@
         <v>28</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+        <v>60</v>
+      </c>
+      <c r="F28" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="J28" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="O28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P28" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="Q28" s="19"/>
       <c r="R28" s="20"/>
-      <c r="S28" s="35"/>
+      <c r="S28" s="35" t="s">
+        <v>177</v>
+      </c>
       <c r="T28" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>25</v>
@@ -4005,22 +4047,22 @@
         <v>28</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F29" s="17">
-        <v>44995</v>
+        <v>44994</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>40</v>
@@ -4033,7 +4075,7 @@
         <v>40</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O29" s="19" t="s">
         <v>40</v>
@@ -4044,15 +4086,15 @@
       <c r="Q29" s="19"/>
       <c r="R29" s="20"/>
       <c r="S29" s="35" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="T29" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>25</v>
@@ -4061,36 +4103,54 @@
         <v>28</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="F30" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>152</v>
+      </c>
       <c r="J30" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="O30" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P30" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="Q30" s="19"/>
       <c r="R30" s="20"/>
-      <c r="S30" s="35"/>
+      <c r="S30" s="35" t="s">
+        <v>151</v>
+      </c>
       <c r="T30" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>25</v>
@@ -4099,36 +4159,54 @@
         <v>28</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
+        <v>66</v>
+      </c>
+      <c r="F31" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="J31" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M31" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N31" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="O31" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="Q31" s="19"/>
       <c r="R31" s="20"/>
-      <c r="S31" s="35"/>
+      <c r="S31" s="35" t="s">
+        <v>155</v>
+      </c>
       <c r="T31" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>25</v>
@@ -4137,10 +4215,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
@@ -4150,7 +4228,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -4164,9 +4242,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>25</v>
@@ -4175,36 +4253,54 @@
         <v>28</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="F33" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>174</v>
+      </c>
       <c r="J33" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N33" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="O33" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P33" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="Q33" s="19"/>
       <c r="R33" s="20"/>
-      <c r="S33" s="35"/>
+      <c r="S33" s="35" t="s">
+        <v>173</v>
+      </c>
       <c r="T33" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>25</v>
@@ -4213,10 +4309,10 @@
         <v>28</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4226,7 +4322,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
@@ -4240,9 +4336,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>25</v>
@@ -4251,118 +4347,202 @@
         <v>28</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G35" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="I35" s="18" t="s">
-        <v>168</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
       <c r="J35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="O35" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P35" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
       <c r="R35" s="20"/>
-      <c r="S35" s="35" t="s">
-        <v>166</v>
-      </c>
+      <c r="S35" s="35"/>
       <c r="T35" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="31"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="34"/>
-      <c r="T37" s="31"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="31"/>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="31"/>
+    <row r="36" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>90</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="20"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>91</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
+        <v>92</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>93</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="O39" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P39" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="20"/>
+      <c r="S39" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="T39" s="30" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F40" s="7"/>
@@ -17811,8 +17991,76 @@
       <c r="S830" s="34"/>
       <c r="T830" s="31"/>
     </row>
+    <row r="831" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F831" s="7"/>
+      <c r="G831" s="7"/>
+      <c r="H831" s="7"/>
+      <c r="I831" s="7"/>
+      <c r="J831" s="8"/>
+      <c r="K831" s="8"/>
+      <c r="L831" s="8"/>
+      <c r="M831" s="8"/>
+      <c r="N831" s="8"/>
+      <c r="O831" s="8"/>
+      <c r="P831" s="8"/>
+      <c r="Q831" s="8"/>
+      <c r="R831" s="9"/>
+      <c r="S831" s="34"/>
+      <c r="T831" s="31"/>
+    </row>
+    <row r="832" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F832" s="7"/>
+      <c r="G832" s="7"/>
+      <c r="H832" s="7"/>
+      <c r="I832" s="7"/>
+      <c r="J832" s="8"/>
+      <c r="K832" s="8"/>
+      <c r="L832" s="8"/>
+      <c r="M832" s="8"/>
+      <c r="N832" s="8"/>
+      <c r="O832" s="8"/>
+      <c r="P832" s="8"/>
+      <c r="Q832" s="8"/>
+      <c r="R832" s="9"/>
+      <c r="S832" s="34"/>
+      <c r="T832" s="31"/>
+    </row>
+    <row r="833" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F833" s="7"/>
+      <c r="G833" s="7"/>
+      <c r="H833" s="7"/>
+      <c r="I833" s="7"/>
+      <c r="J833" s="8"/>
+      <c r="K833" s="8"/>
+      <c r="L833" s="8"/>
+      <c r="M833" s="8"/>
+      <c r="N833" s="8"/>
+      <c r="O833" s="8"/>
+      <c r="P833" s="8"/>
+      <c r="Q833" s="8"/>
+      <c r="R833" s="9"/>
+      <c r="S833" s="34"/>
+      <c r="T833" s="31"/>
+    </row>
+    <row r="834" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F834" s="7"/>
+      <c r="G834" s="7"/>
+      <c r="H834" s="7"/>
+      <c r="I834" s="7"/>
+      <c r="J834" s="8"/>
+      <c r="K834" s="8"/>
+      <c r="L834" s="8"/>
+      <c r="M834" s="8"/>
+      <c r="N834" s="8"/>
+      <c r="O834" s="8"/>
+      <c r="P834" s="8"/>
+      <c r="Q834" s="8"/>
+      <c r="R834" s="9"/>
+      <c r="S834" s="34"/>
+      <c r="T834" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:T35" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A9:T39" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -17832,19 +18080,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J10:J35</xm:sqref>
+          <xm:sqref>J14:J39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q10:Q35</xm:sqref>
+          <xm:sqref>Q14:Q39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{172AE6BC-1BED-4065-86D7-76D10C9574F5}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:M8 O1:O8 L10:M1048576 O10:O1048576</xm:sqref>
+          <xm:sqref>L1:M8 O1:O8 L14:M1048576 O14:O1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -20052,27 +20300,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -20322,34 +20549,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
-    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20369,6 +20590,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
+    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
EBIT Srl invio filesper Accreditamento LDO
inviati in un'unica cartella, comprensiva adesso dei casi RAD e LDO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E088FC-F6DE-43E8-889E-363C3FBED9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88629F1-92EF-4BE3-B02B-AAD055A27399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="28875" windowHeight="15480" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="259">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -980,6 +980,232 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt mancante di campi obbligatori, quindi non valido.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario non valorizzare nel JWT il campo "purpose_of_use".</t>
+    </r>
+  </si>
+  <si>
+    <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Precondizioni:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Il fornitore utilizza un token jwt con dei campi valorizzati in maniera errata.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Descrizione di Business del caso di test: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt avente dei campi valorizzati in maniera errata al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Al fine di rendere non valido il token è necessario valorizzare il campo "action_id" con la stringa "TEST" (valore non ammesso).</t>
+    </r>
+  </si>
+  <si>
+    <t>VALIDAZIONE_LDO_TIMEOUT</t>
+  </si>
+  <si>
+    <t>Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
+"ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT5_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT6_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT7_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT8_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT9_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT10_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT11_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT12_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT13_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT15_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>VALIDAZIONE_CDA2_LDO_CT16_KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.cc9bcd6875060ec6e226bea3c782b9fd441a12d842216e08d124e98a7209506b.d956583c46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f1610a21dd877f95</t>
+  </si>
+  <si>
+    <t>2023-09-26T16:26:24.763Z</t>
+  </si>
+  <si>
+    <t>il periodo di somministrazione della terapia non è gestito dall'applicativo</t>
+  </si>
+  <si>
+    <t>la codifica della terapia non è gestita dall'applicativo</t>
+  </si>
+  <si>
+    <t>il campo è obbligatorio nel motore di integrazione con i valori V e N</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.b3dbd14480730adfa769a826b526e075250defcea4ceb99a8e15b7cf965ee8af.d65d7313c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3cb31331a2a71b56</t>
+  </si>
+  <si>
+    <t>Errore vocabolario. Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.6.103, Codes: CodiceErrato]</t>
+  </si>
+  <si>
+    <t>2023-09-27T17:17:00.600Z</t>
+  </si>
+  <si>
+    <t>il riferimento temporale per distinguere naamnesi prossima da remota non è gestito dall'applicativo</t>
+  </si>
 </sst>
 </file>
 
@@ -988,7 +1214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1091,6 +1317,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1445,28 +1678,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1493,6 +1704,28 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2937,13 +3170,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T834"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T849"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,9 +3188,9 @@
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
     <col min="6" max="9" width="33.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" customWidth="1"/>
     <col min="11" max="15" width="36.42578125" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" customWidth="1"/>
+    <col min="16" max="16" width="55.85546875" customWidth="1"/>
     <col min="17" max="17" width="33.140625" customWidth="1"/>
     <col min="18" max="18" width="36.42578125" customWidth="1"/>
     <col min="19" max="19" width="31.85546875" style="36" customWidth="1"/>
@@ -2983,14 +3217,14 @@
       <c r="T1" s="31"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="40"/>
+      <c r="D2" s="49"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -3008,14 +3242,14 @@
       <c r="T2" s="31"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="49"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -3033,12 +3267,12 @@
       <c r="T3" s="31"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -3057,12 +3291,12 @@
       <c r="T4" s="31"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="49"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -3080,8 +3314,8 @@
       <c r="T5" s="31"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -3199,166 +3433,176 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49">
+      <c r="A10" s="37">
         <v>6</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="40">
         <v>45189</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="J10" s="54" t="s">
+      <c r="J10" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="57" t="s">
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49">
+      <c r="A11" s="37">
         <v>7</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="54" t="s">
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="K11" s="54" t="s">
+      <c r="K11" s="42" t="s">
         <v>210</v>
       </c>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="57" t="s">
+      <c r="L11" s="42"/>
+      <c r="M11" s="42"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49">
+      <c r="A12" s="37">
         <v>8</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="40">
         <v>45189</v>
       </c>
-      <c r="G12" s="53" t="s">
+      <c r="G12" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="H12" s="53" t="s">
+      <c r="H12" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="57" t="s">
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="45" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49">
+      <c r="A13" s="37">
         <v>9</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="F13" s="52"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="54"/>
-      <c r="P13" s="54"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="57" t="s">
+      <c r="F13" s="40">
+        <v>45195</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>250</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="42"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="45" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>11</v>
       </c>
@@ -3402,7 +3646,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>12</v>
       </c>
@@ -3446,7 +3690,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>13</v>
       </c>
@@ -3484,7 +3728,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>14</v>
       </c>
@@ -3523,46 +3767,46 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>31</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="37">
+        <v>29</v>
+      </c>
+      <c r="B18" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="C18" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
       <c r="J18" s="19" t="s">
         <v>100</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="30" t="s">
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>25</v>
@@ -3571,10 +3815,10 @@
         <v>28</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
@@ -3598,9 +3842,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>25</v>
@@ -3609,118 +3853,118 @@
         <v>28</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>127</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" s="19"/>
+        <v>100</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>191</v>
+      </c>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
-      <c r="N20" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="O20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>178</v>
-      </c>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
-      <c r="R20" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="R20" s="20"/>
       <c r="S20" s="35"/>
       <c r="T20" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>75</v>
-      </c>
-      <c r="B21" s="15" t="s">
+    <row r="21" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="37">
+        <v>37</v>
+      </c>
+      <c r="B21" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="C21" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
       <c r="J21" s="19" t="s">
         <v>100</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>76</v>
-      </c>
-      <c r="B22" s="15" t="s">
+    <row r="22" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="37">
+        <v>45</v>
+      </c>
+      <c r="B22" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="15" t="s">
+      <c r="C22" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="44"/>
+      <c r="T22" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
         <v>47</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>77</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>25</v>
@@ -3729,654 +3973,514 @@
         <v>28</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>144</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
       <c r="J23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="K23" s="19"/>
-      <c r="L23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
       <c r="N23" s="19" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="O23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="Q23" s="19"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="35" t="s">
-        <v>131</v>
-      </c>
+      <c r="R23" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="S23" s="35"/>
       <c r="T23" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>78</v>
-      </c>
-      <c r="B24" s="15" t="s">
+    <row r="24" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="37">
+        <v>63</v>
+      </c>
+      <c r="B24" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19" t="s">
+      <c r="C24" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="42" t="s">
         <v>100</v>
       </c>
       <c r="K24" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="37">
+        <v>64</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="37">
+        <v>65</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="37">
+        <v>66</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="F27" s="40"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K27" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="30" t="s">
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>79</v>
-      </c>
-      <c r="B25" s="15" t="s">
+    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="37">
+        <v>67</v>
+      </c>
+      <c r="B28" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="J25" s="19" t="s">
+      <c r="C28" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="37">
+        <v>68</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>234</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="37">
+        <v>69</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="44"/>
+      <c r="T30" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="37">
+        <v>70</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="44"/>
+      <c r="T31" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="37">
+        <v>71</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="40"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="44"/>
+      <c r="T32" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="37">
+        <v>72</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="F33" s="40"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="44"/>
+      <c r="T33" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="37">
+        <v>73</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>245</v>
+      </c>
+      <c r="F34" s="40">
+        <v>45196</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="H34" s="41" t="s">
+        <v>255</v>
+      </c>
+      <c r="I34" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="J34" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19" t="s">
+      <c r="K34" s="42"/>
+      <c r="L34" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="M25" s="19" t="s">
+      <c r="M34" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="N25" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="O25" s="19" t="s">
+      <c r="N34" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="O34" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="P25" s="19" t="s">
+      <c r="P34" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="T25" s="30" t="s">
+      <c r="Q34" s="42"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="44"/>
+      <c r="T34" s="45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>80</v>
-      </c>
-      <c r="B26" s="15" t="s">
+    <row r="35" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="37">
+        <v>74</v>
+      </c>
+      <c r="B35" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N26" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="O26" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P26" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="T26" s="30" t="s">
+      <c r="C35" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="F35" s="40"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>81</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M27" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="O27" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P27" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="T27" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>82</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G28" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="J28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="O28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P28" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="T28" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
-        <v>83</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="J29" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M29" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N29" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="O29" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P29" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="20"/>
-      <c r="S29" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="T29" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
-        <v>84</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="H30" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="J30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N30" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="O30" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P30" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="T30" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
-        <v>85</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="17">
-        <v>44994</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M31" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N31" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="O31" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P31" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="T31" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
-        <v>86</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
-        <v>87</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="J33" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M33" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N33" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="O33" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P33" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="35" t="s">
-        <v>173</v>
-      </c>
-      <c r="T33" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
-        <v>88</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
-        <v>89</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="35"/>
-      <c r="T35" s="30" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>25</v>
@@ -4385,10 +4489,10 @@
         <v>28</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
@@ -4398,7 +4502,7 @@
         <v>100</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="L36" s="19"/>
       <c r="M36" s="19"/>
@@ -4412,9 +4516,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>25</v>
@@ -4423,10 +4527,10 @@
         <v>28</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
@@ -4436,7 +4540,7 @@
         <v>100</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="L37" s="19"/>
       <c r="M37" s="19"/>
@@ -4450,9 +4554,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>25</v>
@@ -4461,36 +4565,54 @@
         <v>28</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
+        <v>50</v>
+      </c>
+      <c r="F38" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="J38" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="K38" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N38" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="O38" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P38" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="Q38" s="19"/>
       <c r="R38" s="20"/>
-      <c r="S38" s="35"/>
+      <c r="S38" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="T38" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>25</v>
@@ -4499,307 +4621,766 @@
         <v>28</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="17">
-        <v>44995</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="H39" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>168</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
       <c r="J39" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="M39" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="N39" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="O39" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="P39" s="19" t="s">
-        <v>192</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
       <c r="Q39" s="19"/>
       <c r="R39" s="20"/>
-      <c r="S39" s="35" t="s">
-        <v>166</v>
-      </c>
+      <c r="S39" s="35"/>
       <c r="T39" s="30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="8"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="31"/>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-      <c r="O41" s="8"/>
-      <c r="P41" s="8"/>
-      <c r="Q41" s="8"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="34"/>
-      <c r="T41" s="31"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="8"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="34"/>
-      <c r="T42" s="31"/>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="34"/>
-      <c r="T43" s="31"/>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="34"/>
-      <c r="T44" s="31"/>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="34"/>
-      <c r="T45" s="31"/>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="34"/>
-      <c r="T46" s="31"/>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="34"/>
-      <c r="T47" s="31"/>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="34"/>
-      <c r="T48" s="31"/>
-    </row>
-    <row r="49" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="8"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="34"/>
-      <c r="T49" s="31"/>
-    </row>
-    <row r="50" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="9"/>
-      <c r="S50" s="34"/>
-      <c r="T50" s="31"/>
-    </row>
-    <row r="51" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="Q51" s="8"/>
-      <c r="R51" s="9"/>
-      <c r="S51" s="34"/>
-      <c r="T51" s="31"/>
-    </row>
-    <row r="52" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="I52" s="7"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="Q52" s="8"/>
-      <c r="R52" s="9"/>
-      <c r="S52" s="34"/>
-      <c r="T52" s="31"/>
-    </row>
-    <row r="53" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="9"/>
-      <c r="S53" s="34"/>
-      <c r="T53" s="31"/>
-    </row>
-    <row r="54" spans="6:20" x14ac:dyDescent="0.25">
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-      <c r="Q54" s="8"/>
-      <c r="R54" s="9"/>
-      <c r="S54" s="34"/>
-      <c r="T54" s="31"/>
-    </row>
-    <row r="55" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>79</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N40" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="O40" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P40" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="T40" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>80</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N41" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="O41" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P41" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="T41" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>81</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F42" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="O42" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P42" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="T42" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>82</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="O43" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P43" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="T43" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>83</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N44" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="O44" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="T44" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>84</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="I45" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N45" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="O45" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P45" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="T45" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>85</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" s="17">
+        <v>44994</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N46" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="O46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P46" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="20"/>
+      <c r="S46" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="T46" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>86</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K47" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="35"/>
+      <c r="T47" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>87</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="I48" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="J48" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M48" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N48" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="O48" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P48" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="20"/>
+      <c r="S48" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="T48" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>88</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="17"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>89</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" s="17"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K50" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="20"/>
+      <c r="S50" s="35"/>
+      <c r="T50" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>90</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F51" s="17"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K51" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="35"/>
+      <c r="T51" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>91</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="17"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="20"/>
+      <c r="S52" s="35"/>
+      <c r="T52" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>92</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="K53" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="35"/>
+      <c r="T53" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>93</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F54" s="17">
+        <v>44995</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="I54" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="J54" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M54" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N54" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="O54" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P54" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="T54" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -4816,7 +5397,7 @@
       <c r="S55" s="34"/>
       <c r="T55" s="31"/>
     </row>
-    <row r="56" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -4833,7 +5414,7 @@
       <c r="S56" s="34"/>
       <c r="T56" s="31"/>
     </row>
-    <row r="57" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -4850,7 +5431,7 @@
       <c r="S57" s="34"/>
       <c r="T57" s="31"/>
     </row>
-    <row r="58" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -4867,7 +5448,7 @@
       <c r="S58" s="34"/>
       <c r="T58" s="31"/>
     </row>
-    <row r="59" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -4884,7 +5465,7 @@
       <c r="S59" s="34"/>
       <c r="T59" s="31"/>
     </row>
-    <row r="60" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
@@ -4901,7 +5482,7 @@
       <c r="S60" s="34"/>
       <c r="T60" s="31"/>
     </row>
-    <row r="61" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
@@ -4918,7 +5499,7 @@
       <c r="S61" s="34"/>
       <c r="T61" s="31"/>
     </row>
-    <row r="62" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
@@ -4935,7 +5516,7 @@
       <c r="S62" s="34"/>
       <c r="T62" s="31"/>
     </row>
-    <row r="63" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
@@ -4952,7 +5533,7 @@
       <c r="S63" s="34"/>
       <c r="T63" s="31"/>
     </row>
-    <row r="64" spans="6:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
@@ -18059,8 +18640,269 @@
       <c r="S834" s="34"/>
       <c r="T834" s="31"/>
     </row>
+    <row r="835" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F835" s="7"/>
+      <c r="G835" s="7"/>
+      <c r="H835" s="7"/>
+      <c r="I835" s="7"/>
+      <c r="J835" s="8"/>
+      <c r="K835" s="8"/>
+      <c r="L835" s="8"/>
+      <c r="M835" s="8"/>
+      <c r="N835" s="8"/>
+      <c r="O835" s="8"/>
+      <c r="P835" s="8"/>
+      <c r="Q835" s="8"/>
+      <c r="R835" s="9"/>
+      <c r="S835" s="34"/>
+      <c r="T835" s="31"/>
+    </row>
+    <row r="836" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F836" s="7"/>
+      <c r="G836" s="7"/>
+      <c r="H836" s="7"/>
+      <c r="I836" s="7"/>
+      <c r="J836" s="8"/>
+      <c r="K836" s="8"/>
+      <c r="L836" s="8"/>
+      <c r="M836" s="8"/>
+      <c r="N836" s="8"/>
+      <c r="O836" s="8"/>
+      <c r="P836" s="8"/>
+      <c r="Q836" s="8"/>
+      <c r="R836" s="9"/>
+      <c r="S836" s="34"/>
+      <c r="T836" s="31"/>
+    </row>
+    <row r="837" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F837" s="7"/>
+      <c r="G837" s="7"/>
+      <c r="H837" s="7"/>
+      <c r="I837" s="7"/>
+      <c r="J837" s="8"/>
+      <c r="K837" s="8"/>
+      <c r="L837" s="8"/>
+      <c r="M837" s="8"/>
+      <c r="N837" s="8"/>
+      <c r="O837" s="8"/>
+      <c r="P837" s="8"/>
+      <c r="Q837" s="8"/>
+      <c r="R837" s="9"/>
+      <c r="S837" s="34"/>
+      <c r="T837" s="31"/>
+    </row>
+    <row r="838" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F838" s="7"/>
+      <c r="G838" s="7"/>
+      <c r="H838" s="7"/>
+      <c r="I838" s="7"/>
+      <c r="J838" s="8"/>
+      <c r="K838" s="8"/>
+      <c r="L838" s="8"/>
+      <c r="M838" s="8"/>
+      <c r="N838" s="8"/>
+      <c r="O838" s="8"/>
+      <c r="P838" s="8"/>
+      <c r="Q838" s="8"/>
+      <c r="R838" s="9"/>
+      <c r="S838" s="34"/>
+      <c r="T838" s="31"/>
+    </row>
+    <row r="839" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F839" s="7"/>
+      <c r="G839" s="7"/>
+      <c r="H839" s="7"/>
+      <c r="I839" s="7"/>
+      <c r="J839" s="8"/>
+      <c r="K839" s="8"/>
+      <c r="L839" s="8"/>
+      <c r="M839" s="8"/>
+      <c r="N839" s="8"/>
+      <c r="O839" s="8"/>
+      <c r="P839" s="8"/>
+      <c r="Q839" s="8"/>
+      <c r="R839" s="9"/>
+      <c r="S839" s="34"/>
+      <c r="T839" s="31"/>
+    </row>
+    <row r="840" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F840" s="7"/>
+      <c r="G840" s="7"/>
+      <c r="H840" s="7"/>
+      <c r="I840" s="7"/>
+      <c r="J840" s="8"/>
+      <c r="K840" s="8"/>
+      <c r="L840" s="8"/>
+      <c r="M840" s="8"/>
+      <c r="N840" s="8"/>
+      <c r="O840" s="8"/>
+      <c r="P840" s="8"/>
+      <c r="Q840" s="8"/>
+      <c r="R840" s="9"/>
+      <c r="S840" s="34"/>
+      <c r="T840" s="31"/>
+    </row>
+    <row r="841" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F841" s="7"/>
+      <c r="G841" s="7"/>
+      <c r="H841" s="7"/>
+      <c r="I841" s="7"/>
+      <c r="J841" s="8"/>
+      <c r="K841" s="8"/>
+      <c r="L841" s="8"/>
+      <c r="M841" s="8"/>
+      <c r="N841" s="8"/>
+      <c r="O841" s="8"/>
+      <c r="P841" s="8"/>
+      <c r="Q841" s="8"/>
+      <c r="R841" s="9"/>
+      <c r="S841" s="34"/>
+      <c r="T841" s="31"/>
+    </row>
+    <row r="842" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F842" s="7"/>
+      <c r="G842" s="7"/>
+      <c r="H842" s="7"/>
+      <c r="I842" s="7"/>
+      <c r="J842" s="8"/>
+      <c r="K842" s="8"/>
+      <c r="L842" s="8"/>
+      <c r="M842" s="8"/>
+      <c r="N842" s="8"/>
+      <c r="O842" s="8"/>
+      <c r="P842" s="8"/>
+      <c r="Q842" s="8"/>
+      <c r="R842" s="9"/>
+      <c r="S842" s="34"/>
+      <c r="T842" s="31"/>
+    </row>
+    <row r="843" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F843" s="7"/>
+      <c r="G843" s="7"/>
+      <c r="H843" s="7"/>
+      <c r="I843" s="7"/>
+      <c r="J843" s="8"/>
+      <c r="K843" s="8"/>
+      <c r="L843" s="8"/>
+      <c r="M843" s="8"/>
+      <c r="N843" s="8"/>
+      <c r="O843" s="8"/>
+      <c r="P843" s="8"/>
+      <c r="Q843" s="8"/>
+      <c r="R843" s="9"/>
+      <c r="S843" s="34"/>
+      <c r="T843" s="31"/>
+    </row>
+    <row r="844" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F844" s="7"/>
+      <c r="G844" s="7"/>
+      <c r="H844" s="7"/>
+      <c r="I844" s="7"/>
+      <c r="J844" s="8"/>
+      <c r="K844" s="8"/>
+      <c r="L844" s="8"/>
+      <c r="M844" s="8"/>
+      <c r="N844" s="8"/>
+      <c r="O844" s="8"/>
+      <c r="P844" s="8"/>
+      <c r="Q844" s="8"/>
+      <c r="R844" s="9"/>
+      <c r="S844" s="34"/>
+      <c r="T844" s="31"/>
+    </row>
+    <row r="845" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F845" s="7"/>
+      <c r="G845" s="7"/>
+      <c r="H845" s="7"/>
+      <c r="I845" s="7"/>
+      <c r="J845" s="8"/>
+      <c r="K845" s="8"/>
+      <c r="L845" s="8"/>
+      <c r="M845" s="8"/>
+      <c r="N845" s="8"/>
+      <c r="O845" s="8"/>
+      <c r="P845" s="8"/>
+      <c r="Q845" s="8"/>
+      <c r="R845" s="9"/>
+      <c r="S845" s="34"/>
+      <c r="T845" s="31"/>
+    </row>
+    <row r="846" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F846" s="7"/>
+      <c r="G846" s="7"/>
+      <c r="H846" s="7"/>
+      <c r="I846" s="7"/>
+      <c r="J846" s="8"/>
+      <c r="K846" s="8"/>
+      <c r="L846" s="8"/>
+      <c r="M846" s="8"/>
+      <c r="N846" s="8"/>
+      <c r="O846" s="8"/>
+      <c r="P846" s="8"/>
+      <c r="Q846" s="8"/>
+      <c r="R846" s="9"/>
+      <c r="S846" s="34"/>
+      <c r="T846" s="31"/>
+    </row>
+    <row r="847" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F847" s="7"/>
+      <c r="G847" s="7"/>
+      <c r="H847" s="7"/>
+      <c r="I847" s="7"/>
+      <c r="J847" s="8"/>
+      <c r="K847" s="8"/>
+      <c r="L847" s="8"/>
+      <c r="M847" s="8"/>
+      <c r="N847" s="8"/>
+      <c r="O847" s="8"/>
+      <c r="P847" s="8"/>
+      <c r="Q847" s="8"/>
+      <c r="R847" s="9"/>
+      <c r="S847" s="34"/>
+      <c r="T847" s="31"/>
+    </row>
+    <row r="848" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F848" s="7"/>
+      <c r="G848" s="7"/>
+      <c r="H848" s="7"/>
+      <c r="I848" s="7"/>
+      <c r="J848" s="8"/>
+      <c r="K848" s="8"/>
+      <c r="L848" s="8"/>
+      <c r="M848" s="8"/>
+      <c r="N848" s="8"/>
+      <c r="O848" s="8"/>
+      <c r="P848" s="8"/>
+      <c r="Q848" s="8"/>
+      <c r="R848" s="9"/>
+      <c r="S848" s="34"/>
+      <c r="T848" s="31"/>
+    </row>
+    <row r="849" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F849" s="7"/>
+      <c r="G849" s="7"/>
+      <c r="H849" s="7"/>
+      <c r="I849" s="7"/>
+      <c r="J849" s="8"/>
+      <c r="K849" s="8"/>
+      <c r="L849" s="8"/>
+      <c r="M849" s="8"/>
+      <c r="N849" s="8"/>
+      <c r="O849" s="8"/>
+      <c r="P849" s="8"/>
+      <c r="Q849" s="8"/>
+      <c r="R849" s="9"/>
+      <c r="S849" s="34"/>
+      <c r="T849" s="31"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A9:T39" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A9:T54" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="LDO"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -18080,19 +18922,19 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14:J39</xm:sqref>
+          <xm:sqref>J14:J21 J23 J36:J54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Sheet1!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>Q14:Q39</xm:sqref>
+          <xm:sqref>Q14:Q17 Q19:Q20 Q23 Q36:Q54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{172AE6BC-1BED-4065-86D7-76D10C9574F5}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:M8 O1:O8 L14:M1048576 O14:O1048576</xm:sqref>
+          <xm:sqref>L1:M8 O1:O8 O36:O1048576 O14:O17 L14:M17 L19:M20 O19:O20 O23 L23:M23 L36:M1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -20300,6 +21142,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -20549,28 +21412,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
+    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20590,33 +21459,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
-    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
EBITSRL invio file per correzione campi opzionali
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88629F1-92EF-4BE3-B02B-AAD055A27399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C0E0F9-6E30-4C97-905F-784B5FC2C6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28560" yWindow="0" windowWidth="29040" windowHeight="15480" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="255">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -936,15 +936,6 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-09-20T15:42:36.960Z</t>
-  </si>
-  <si>
-    <t>ba744235c0982da3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.a8a52ff8607a2e5ed11b83cb04d452bf3a9ed38d6e681f109347757dd84edfd9.0061e771fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT2</t>
   </si>
   <si>
@@ -962,15 +953,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-09-20T17:23:39.103Z</t>
-  </si>
-  <si>
-    <t>0cb7f69dd5903495</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.f57eaf84fca19f8a37acfbc97d9312c3131f1f1e6c7bdb0fd3955da4cb4bfaa7.3417077500^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -1174,15 +1156,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.cc9bcd6875060ec6e226bea3c782b9fd441a12d842216e08d124e98a7209506b.d956583c46^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f1610a21dd877f95</t>
-  </si>
-  <si>
-    <t>2023-09-26T16:26:24.763Z</t>
-  </si>
-  <si>
     <t>il periodo di somministrazione della terapia non è gestito dall'applicativo</t>
   </si>
   <si>
@@ -1204,7 +1177,22 @@
     <t>2023-09-27T17:17:00.600Z</t>
   </si>
   <si>
-    <t>il riferimento temporale per distinguere naamnesi prossima da remota non è gestito dall'applicativo</t>
+    <t>2023-09-29T13:13:13.800Z</t>
+  </si>
+  <si>
+    <t>9ff67298181124b5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.97882b29e1e1a8634253aae9af10816b882260dfbc671c1010ee55c69868af42.1dd9958328^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>il riferimento temporale per distinguere anamnesi prossima da remota non è gestito dall'applicativo</t>
+  </si>
+  <si>
+    <t>alcuni dettagli non vengono trattati separatamente dall'applicativo</t>
+  </si>
+  <si>
+    <t>alcuni dettagli opzionali non vengono trattati separatamente dall'applicativo</t>
   </si>
 </sst>
 </file>
@@ -3174,10 +3162,10 @@
   <dimension ref="A1:T849"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3449,16 +3437,16 @@
         <v>204</v>
       </c>
       <c r="F10" s="40">
-        <v>45189</v>
+        <v>45198</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="J10" s="42" t="s">
         <v>40</v>
@@ -3487,10 +3475,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F11" s="40"/>
       <c r="G11" s="41"/>
@@ -3500,7 +3488,7 @@
         <v>100</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L11" s="42"/>
       <c r="M11" s="42"/>
@@ -3525,27 +3513,21 @@
         <v>27</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>212</v>
-      </c>
-      <c r="F12" s="40">
-        <v>45189</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="41" t="s">
-        <v>215</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="42"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>253</v>
+      </c>
       <c r="L12" s="42"/>
       <c r="M12" s="42"/>
       <c r="N12" s="42"/>
@@ -3569,27 +3551,21 @@
         <v>27</v>
       </c>
       <c r="D13" s="38" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>217</v>
-      </c>
-      <c r="F13" s="40">
-        <v>45195</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>250</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="I13" s="41" t="s">
-        <v>248</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="42"/>
+        <v>100</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>254</v>
+      </c>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
@@ -3777,10 +3753,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="41"/>
@@ -3891,10 +3867,10 @@
         <v>27</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="41"/>
@@ -3929,10 +3905,10 @@
         <v>27</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F22" s="40"/>
       <c r="G22" s="41"/>
@@ -4017,10 +3993,10 @@
         <v>27</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="F24" s="40"/>
       <c r="G24" s="41"/>
@@ -4055,10 +4031,10 @@
         <v>27</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="41"/>
@@ -4093,10 +4069,10 @@
         <v>27</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F26" s="40"/>
       <c r="G26" s="41"/>
@@ -4106,7 +4082,7 @@
         <v>100</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="L26" s="42"/>
       <c r="M26" s="42"/>
@@ -4131,10 +4107,10 @@
         <v>27</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="41"/>
@@ -4169,10 +4145,10 @@
         <v>27</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
@@ -4207,10 +4183,10 @@
         <v>27</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="F29" s="40"/>
       <c r="G29" s="41"/>
@@ -4245,10 +4221,10 @@
         <v>27</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F30" s="40"/>
       <c r="G30" s="41"/>
@@ -4283,10 +4259,10 @@
         <v>27</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="F31" s="40"/>
       <c r="G31" s="41"/>
@@ -4321,10 +4297,10 @@
         <v>27</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F32" s="40"/>
       <c r="G32" s="41"/>
@@ -4334,7 +4310,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="L32" s="42"/>
       <c r="M32" s="42"/>
@@ -4359,10 +4335,10 @@
         <v>27</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F33" s="40"/>
       <c r="G33" s="41"/>
@@ -4372,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="L33" s="42"/>
       <c r="M33" s="42"/>
@@ -4397,22 +4373,22 @@
         <v>27</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="F34" s="40">
         <v>45196</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="H34" s="41" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="J34" s="42" t="s">
         <v>40</v>
@@ -4425,7 +4401,7 @@
         <v>40</v>
       </c>
       <c r="N34" s="42" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="O34" s="42" t="s">
         <v>40</v>
@@ -4451,10 +4427,10 @@
         <v>27</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="F35" s="40"/>
       <c r="G35" s="41"/>
@@ -4464,7 +4440,7 @@
         <v>100</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="L35" s="42"/>
       <c r="M35" s="42"/>
@@ -21142,27 +21118,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001C548C50377FF94DA5992E79C7BD108D" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="79da61cccba856d26d04def5fd5409fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xmlns:ns3="74204614-352d-415a-b69e-46d10468735d" xmlns:ns4="e1629bc7-f521-4968-9d85-8991e5c0d15e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb6e121baa4fd234d2adc618a44a0dc9" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
@@ -21412,34 +21367,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
-    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DFF6DC8-B71B-416A-B7FD-9F7BDC6DDC7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21459,6 +21408,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e1629bc7-f521-4968-9d85-8991e5c0d15e"/>
+    <ds:schemaRef ds:uri="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Accreditamento LDO EBIT Srl
Update report-checklist per accreditamento LDO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A975963-3B3C-4650-A50C-F930819EB1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8BDE0D-5D59-4A54-B162-934BC70C54C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28560" yWindow="0" windowWidth="29040" windowHeight="15480" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="1170" windowWidth="21600" windowHeight="11295" tabRatio="424" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -3165,7 +3165,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21368,15 +21368,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="e1629bc7-f521-4968-9d85-8991e5c0d15e" xsi:nil="true"/>
@@ -21386,6 +21377,15 @@
     <Descrizione xmlns="4b14fa8f-0c88-4113-956d-8f7b7d25bf6d" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21409,14 +21409,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -21435,6 +21427,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Accreditamento EBIT Srl LDO RAD RSA
modificato il caso 147 come indicato via mail
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918FE03-3846-4590-BBFA-E3A607C70BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947536E4-3452-43CA-9817-F4F98525ADBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-1860" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57255" yWindow="-1740" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -3262,15 +3262,6 @@
     <t>la sezione observation/value relativa alle diagnosi non è gestita dall'applicativo</t>
   </si>
   <si>
-    <t>2023-11-10T15:32:48.090Z</t>
-  </si>
-  <si>
-    <t>40d07fc652aa9928</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.10.3.1.4.4.85426c270db34674e48ca78ecae30496cbdffdbe67573888bc125f41c14db920.d11696f361^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>l'applicativo non gestisce esami di tipo ginecologico, ma cardiologico</t>
   </si>
   <si>
@@ -3522,6 +3513,15 @@
   </si>
   <si>
     <t>2023-11-16T10:08:00.090Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.10.3.1.4.4.928c364e8d88e56821b0d24c1509b1f0f0e9df504fbffc5f5ec8323420ecb16b.1108a76f91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>30c1a3e701b9fda2</t>
+  </si>
+  <si>
+    <t>2023-11-16T18:37:34.977Z</t>
   </si>
 </sst>
 </file>
@@ -6447,10 +6447,10 @@
   <dimension ref="A1:T873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6881,13 +6881,13 @@
         <v>45244</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>80</v>
@@ -6925,13 +6925,13 @@
         <v>45244</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>80</v>
@@ -7112,22 +7112,22 @@
         <v>74</v>
       </c>
       <c r="D20" s="21" t="s">
+        <v>694</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>697</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>700</v>
       </c>
       <c r="F20" s="23">
         <v>45246</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>80</v>
@@ -7140,7 +7140,7 @@
         <v>80</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>80</v>
@@ -7151,7 +7151,7 @@
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
       <c r="S20" s="37" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="T20" s="28" t="s">
         <v>68</v>
@@ -7244,22 +7244,22 @@
         <v>74</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="F23" s="23">
         <v>45246</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>80</v>
@@ -7272,7 +7272,7 @@
         <v>80</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="O23" s="25" t="s">
         <v>80</v>
@@ -7283,7 +7283,7 @@
       <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
       <c r="S23" s="37" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="T23" s="28" t="s">
         <v>68</v>
@@ -7993,7 +7993,7 @@
         <v>595</v>
       </c>
       <c r="K41" s="25" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
@@ -8069,7 +8069,7 @@
         <v>595</v>
       </c>
       <c r="K43" s="25" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
@@ -8107,7 +8107,7 @@
         <v>595</v>
       </c>
       <c r="K44" s="25" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
@@ -8141,13 +8141,13 @@
         <v>45244</v>
       </c>
       <c r="G45" s="24" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="H45" s="24" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>80</v>
@@ -8160,7 +8160,7 @@
         <v>80</v>
       </c>
       <c r="N45" s="25" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="O45" s="25" t="s">
         <v>80</v>
@@ -8171,7 +8171,7 @@
       <c r="Q45" s="25"/>
       <c r="R45" s="26"/>
       <c r="S45" s="37" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="T45" s="28" t="s">
         <v>68</v>
@@ -8197,13 +8197,13 @@
         <v>45244</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>80</v>
@@ -8216,7 +8216,7 @@
         <v>80</v>
       </c>
       <c r="N46" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="O46" s="25" t="s">
         <v>80</v>
@@ -8227,7 +8227,7 @@
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
       <c r="S46" s="37" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="T46" s="28" t="s">
         <v>68</v>
@@ -8257,7 +8257,7 @@
         <v>595</v>
       </c>
       <c r="K47" s="25" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="L47" s="25"/>
       <c r="M47" s="25"/>
@@ -8291,13 +8291,13 @@
         <v>45244</v>
       </c>
       <c r="G48" s="24" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="H48" s="24" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="I48" s="24" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="J48" s="25" t="s">
         <v>80</v>
@@ -8310,7 +8310,7 @@
         <v>80</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>80</v>
@@ -8321,7 +8321,7 @@
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
       <c r="S48" s="37" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="T48" s="28" t="s">
         <v>68</v>
@@ -8351,7 +8351,7 @@
         <v>595</v>
       </c>
       <c r="K49" s="25" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="L49" s="25"/>
       <c r="M49" s="25"/>
@@ -8423,13 +8423,13 @@
         <v>45244</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="J51" s="25" t="s">
         <v>80</v>
@@ -8442,7 +8442,7 @@
         <v>80</v>
       </c>
       <c r="N51" s="25" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="O51" s="25" t="s">
         <v>80</v>
@@ -8453,7 +8453,7 @@
       <c r="Q51" s="25"/>
       <c r="R51" s="26"/>
       <c r="S51" s="37" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="T51" s="28" t="s">
         <v>68</v>
@@ -8669,13 +8669,13 @@
         <v>45244</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="J57" s="25" t="s">
         <v>80</v>
@@ -8688,7 +8688,7 @@
         <v>80</v>
       </c>
       <c r="N57" s="25" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="O57" s="25" t="s">
         <v>80</v>
@@ -8699,7 +8699,7 @@
       <c r="Q57" s="25"/>
       <c r="R57" s="26"/>
       <c r="S57" s="37" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="T57" s="28" t="s">
         <v>68</v>
@@ -8722,16 +8722,16 @@
         <v>147</v>
       </c>
       <c r="F58" s="23">
-        <v>45240</v>
+        <v>45246</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>629</v>
+        <v>708</v>
       </c>
       <c r="H58" s="24" t="s">
-        <v>630</v>
+        <v>707</v>
       </c>
       <c r="I58" s="24" t="s">
-        <v>631</v>
+        <v>706</v>
       </c>
       <c r="J58" s="25" t="s">
         <v>80</v>
@@ -8773,7 +8773,7 @@
         <v>595</v>
       </c>
       <c r="K59" s="25" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="L59" s="25"/>
       <c r="M59" s="25"/>
@@ -8811,7 +8811,7 @@
         <v>595</v>
       </c>
       <c r="K60" s="25" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="L60" s="25"/>
       <c r="M60" s="25"/>
@@ -8849,7 +8849,7 @@
         <v>595</v>
       </c>
       <c r="K61" s="25" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="L61" s="25"/>
       <c r="M61" s="25"/>
@@ -8887,7 +8887,7 @@
         <v>595</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
@@ -8925,7 +8925,7 @@
         <v>595</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
@@ -8963,7 +8963,7 @@
         <v>595</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="L64" s="25"/>
       <c r="M64" s="25"/>
@@ -9039,7 +9039,7 @@
         <v>595</v>
       </c>
       <c r="K66" s="25" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="L66" s="25"/>
       <c r="M66" s="25"/>
@@ -9077,7 +9077,7 @@
         <v>595</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="L67" s="25"/>
       <c r="M67" s="25"/>
@@ -9111,13 +9111,13 @@
         <v>45240</v>
       </c>
       <c r="G68" s="24" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="I68" s="24" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="J68" s="25" t="s">
         <v>80</v>
@@ -9130,7 +9130,7 @@
         <v>80</v>
       </c>
       <c r="N68" s="25" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="O68" s="25" t="s">
         <v>80</v>
@@ -9141,7 +9141,7 @@
       <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
       <c r="S68" s="37" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="T68" s="28" t="s">
         <v>68</v>
@@ -9167,13 +9167,13 @@
         <v>45240</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="H69" s="24" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="I69" s="24" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="J69" s="25" t="s">
         <v>80</v>
@@ -9186,7 +9186,7 @@
         <v>80</v>
       </c>
       <c r="N69" s="25" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="O69" s="25" t="s">
         <v>80</v>
@@ -9225,7 +9225,7 @@
         <v>595</v>
       </c>
       <c r="K70" s="25" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="L70" s="25"/>
       <c r="M70" s="25"/>
@@ -9259,13 +9259,13 @@
         <v>45240</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>80</v>
@@ -9278,7 +9278,7 @@
         <v>80</v>
       </c>
       <c r="N71" s="25" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="O71" s="25" t="s">
         <v>80</v>
@@ -9317,7 +9317,7 @@
         <v>595</v>
       </c>
       <c r="K72" s="25" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="L72" s="25"/>
       <c r="M72" s="25"/>
@@ -9326,7 +9326,7 @@
       <c r="P72" s="25"/>
       <c r="Q72" s="25"/>
       <c r="R72" s="26" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="S72" s="27"/>
       <c r="T72" s="28" t="s">
@@ -9357,14 +9357,14 @@
         <v>595</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="L73" s="25"/>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
       <c r="O73" s="25"/>
       <c r="P73" s="25" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
@@ -9397,14 +9397,14 @@
         <v>595</v>
       </c>
       <c r="K74" s="25" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="L74" s="25"/>
       <c r="M74" s="25"/>
       <c r="N74" s="25"/>
       <c r="O74" s="25"/>
       <c r="P74" s="25" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
@@ -9437,14 +9437,14 @@
         <v>595</v>
       </c>
       <c r="K75" s="25" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="L75" s="25"/>
       <c r="M75" s="25"/>
       <c r="N75" s="25"/>
       <c r="O75" s="25"/>
       <c r="P75" s="25" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
@@ -9477,14 +9477,14 @@
         <v>595</v>
       </c>
       <c r="K76" s="25" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="L76" s="25"/>
       <c r="M76" s="25"/>
       <c r="N76" s="25"/>
       <c r="O76" s="25"/>
       <c r="P76" s="25" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
@@ -9517,14 +9517,14 @@
         <v>595</v>
       </c>
       <c r="K77" s="25" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="L77" s="25"/>
       <c r="M77" s="25"/>
       <c r="N77" s="25"/>
       <c r="O77" s="25"/>
       <c r="P77" s="25" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
@@ -9557,14 +9557,14 @@
         <v>595</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
       <c r="N78" s="25"/>
       <c r="O78" s="25"/>
       <c r="P78" s="25" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="Q78" s="25"/>
       <c r="R78" s="26"/>
@@ -9597,7 +9597,7 @@
         <v>595</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="25"/>
@@ -9635,7 +9635,7 @@
         <v>595</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="25"/>

</xml_diff>

<commit_message>
Accreditamento EBIT Srl RSA LDO
sottoposti nuovamente i casi 37 e 39, 48 e corretto il caso 84, come richiesto via mail.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947536E4-3452-43CA-9817-F4F98525ADBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39303053-0B2B-4C58-8FD8-E7EC851FA51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57255" yWindow="-1740" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="717">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3522,6 +3522,32 @@
   </si>
   <si>
     <t>2023-11-16T18:37:34.977Z</t>
+  </si>
+  <si>
+    <t>Lo stato del record per il quale non è stata completata la trasmissione viene evidenziato all’operatore nella consolle di monitoraggio.
+Nelle evidenze dell’errore viene anche registrato  l'errore ricevuto:
+Errore vocabolario. È stato trovato almeno un dizionario presente in Blocklist: [2.16.840.1.113883.2.9.2.9999.6.11]</t>
+  </si>
+  <si>
+    <t>i valori del @Code e del @CodeSystem nell'entry/act/code dell'esame eseguito,  forzati con valori non consentiti per poter eseguire il test, hanno generato un errore di vocabolario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il motore di integrazione attende un tempo configurabile, passato il quale mostrerà all'utente il messaggio di "connection timeout".  </t>
+  </si>
+  <si>
+    <t>In questo caso l'evento viene inserito in una coda di uscita gestibile dall'utente tramite una consolle di monitoraggio. Il pdf contiene comunque al suo interno il CDA2 per poi essere conferito al FSE in un secondo momento, grazie al riprocessamento dalla consolle di monitoraggio. La coda è configurabile per avvisare automaticamente il nostro Help Desk</t>
+  </si>
+  <si>
+    <t>2023-11-22T13:05:21.160Z</t>
+  </si>
+  <si>
+    <t>3c6c3d34d9883680</t>
+  </si>
+  <si>
+    <t>2023-11-22T14:27:11.190Z</t>
+  </si>
+  <si>
+    <t>f8c14d53682dd9aa</t>
   </si>
 </sst>
 </file>
@@ -6447,10 +6473,10 @@
   <dimension ref="A1:T873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I58" sqref="I58"/>
+      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6624,7 +6650,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -6641,7 +6667,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -6703,7 +6729,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -6747,7 +6773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -6785,7 +6811,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -6823,7 +6849,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -6861,7 +6887,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>11</v>
       </c>
@@ -6905,7 +6931,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>12</v>
       </c>
@@ -6949,7 +6975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>13</v>
       </c>
@@ -6987,7 +7013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>14</v>
       </c>
@@ -7025,7 +7051,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>29</v>
       </c>
@@ -7063,7 +7089,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>31</v>
       </c>
@@ -7173,24 +7199,42 @@
       <c r="E21" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="35" t="s">
-        <v>595</v>
-      </c>
-      <c r="K21" s="35" t="s">
-        <v>606</v>
-      </c>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
+      <c r="F21" s="23">
+        <v>45252</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>716</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>699</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="K21" s="35"/>
+      <c r="L21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N21" s="25" t="s">
+        <v>703</v>
+      </c>
+      <c r="O21" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="P21" s="35" t="s">
+        <v>608</v>
+      </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
-      <c r="S21" s="27"/>
+      <c r="S21" s="37" t="s">
+        <v>702</v>
+      </c>
       <c r="T21" s="28" t="s">
         <v>68</v>
       </c>
@@ -7211,24 +7255,42 @@
       <c r="E22" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+      <c r="F22" s="23">
+        <v>45252</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>713</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>714</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>699</v>
+      </c>
       <c r="J22" s="25" t="s">
-        <v>595</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>606</v>
-      </c>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
+        <v>80</v>
+      </c>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="N22" s="25" t="s">
+        <v>703</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="P22" s="35" t="s">
+        <v>608</v>
+      </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
-      <c r="S22" s="27"/>
+      <c r="S22" s="37" t="s">
+        <v>702</v>
+      </c>
       <c r="T22" s="28" t="s">
         <v>68</v>
       </c>
@@ -7377,7 +7439,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="140.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="20">
         <v>48</v>
       </c>
@@ -7401,16 +7463,20 @@
         <v>80</v>
       </c>
       <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
+      <c r="L26" s="25" t="s">
+        <v>595</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>80</v>
+      </c>
       <c r="N26" s="25" t="s">
-        <v>607</v>
+        <v>711</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>608</v>
+        <v>712</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="26" t="s">
@@ -7421,7 +7487,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>63</v>
       </c>
@@ -7459,7 +7525,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>64</v>
       </c>
@@ -7497,7 +7563,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>65</v>
       </c>
@@ -7535,7 +7601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>66</v>
       </c>
@@ -7573,7 +7639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>67</v>
       </c>
@@ -7611,7 +7677,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
         <v>68</v>
       </c>
@@ -7649,7 +7715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20">
         <v>69</v>
       </c>
@@ -7687,7 +7753,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20">
         <v>70</v>
       </c>
@@ -7725,7 +7791,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20">
         <v>71</v>
       </c>
@@ -7763,7 +7829,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20">
         <v>72</v>
       </c>
@@ -7801,7 +7867,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20">
         <v>73</v>
       </c>
@@ -7855,7 +7921,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20">
         <v>74</v>
       </c>
@@ -7893,7 +7959,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
         <v>75</v>
       </c>
@@ -7931,7 +7997,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20">
         <v>76</v>
       </c>
@@ -7969,7 +8035,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20">
         <v>77</v>
       </c>
@@ -8007,7 +8073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20">
         <v>78</v>
       </c>
@@ -8045,7 +8111,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20">
         <v>79</v>
       </c>
@@ -8083,7 +8149,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20">
         <v>80</v>
       </c>
@@ -8121,7 +8187,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20">
         <v>81</v>
       </c>
@@ -8177,7 +8243,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="20">
         <v>82</v>
       </c>
@@ -8233,7 +8299,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20">
         <v>83</v>
       </c>
@@ -8271,7 +8337,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20">
         <v>84</v>
       </c>
@@ -8310,7 +8376,7 @@
         <v>80</v>
       </c>
       <c r="N48" s="25" t="s">
-        <v>688</v>
+        <v>709</v>
       </c>
       <c r="O48" s="25" t="s">
         <v>80</v>
@@ -8321,13 +8387,13 @@
       <c r="Q48" s="25"/>
       <c r="R48" s="26"/>
       <c r="S48" s="37" t="s">
-        <v>689</v>
+        <v>710</v>
       </c>
       <c r="T48" s="28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20">
         <v>85</v>
       </c>
@@ -8365,7 +8431,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20">
         <v>86</v>
       </c>
@@ -8403,7 +8469,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20">
         <v>87</v>
       </c>
@@ -8459,7 +8525,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20">
         <v>88</v>
       </c>
@@ -8497,7 +8563,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20">
         <v>89</v>
       </c>
@@ -8535,7 +8601,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20">
         <v>90</v>
       </c>
@@ -8573,7 +8639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
         <v>91</v>
       </c>
@@ -8611,7 +8677,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="20">
         <v>92</v>
       </c>
@@ -8649,7 +8715,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="210" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="20">
         <v>93</v>
       </c>
@@ -8705,7 +8771,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="20">
         <v>147</v>
       </c>
@@ -8749,7 +8815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="20">
         <v>148</v>
       </c>
@@ -8787,7 +8853,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20">
         <v>149</v>
       </c>
@@ -8825,7 +8891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="165" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20">
         <v>150</v>
       </c>
@@ -8863,7 +8929,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20">
         <v>151</v>
       </c>
@@ -8901,7 +8967,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20">
         <v>152</v>
       </c>
@@ -8939,7 +9005,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20">
         <v>153</v>
       </c>
@@ -8977,7 +9043,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20">
         <v>154</v>
       </c>
@@ -9015,7 +9081,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20">
         <v>155</v>
       </c>
@@ -9053,7 +9119,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20">
         <v>156</v>
       </c>
@@ -9091,7 +9157,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="20">
         <v>157</v>
       </c>
@@ -9147,7 +9213,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="20">
         <v>158</v>
       </c>
@@ -9201,7 +9267,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="120" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20">
         <v>159</v>
       </c>
@@ -9293,7 +9359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20">
         <v>161</v>
       </c>
@@ -9333,7 +9399,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20">
         <v>162</v>
       </c>
@@ -9373,7 +9439,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20">
         <v>163</v>
       </c>
@@ -9413,7 +9479,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="20">
         <v>164</v>
       </c>
@@ -9453,7 +9519,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20">
         <v>165</v>
       </c>
@@ -9493,7 +9559,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
         <v>166</v>
       </c>
@@ -9533,7 +9599,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="20">
         <v>167</v>
       </c>
@@ -9573,7 +9639,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="20">
         <v>168</v>
       </c>
@@ -9611,7 +9677,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="135" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>169</v>
       </c>
@@ -20289,6 +20355,11 @@
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="SI"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -20311,7 +20382,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14:J15 J41 J51 J43:J49 O47 O49:O50 L49:M50 L52:M56 O52:O56 O38:O45 L38:M45 L47:M47 O10:O23 J66:J80 L58:M80 O58:O80 J57:J64 O26:O36 L10:M36 J24:J26</xm:sqref>
+          <xm:sqref>J14:J15 J41 J51 J43:J49 O47 O49:O50 L49:M50 L52:M56 O52:O56 O38:O45 L38:M45 L47:M47 J66:J80 L58:M80 O58:O80 J57:J64 O26:O36 J24:J26 O10:O23 L10:M36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
Accreditamento EBIT Srl LDO RSA RAD
modificati i casi 37 e 39 secondo quanto richiesto nella mail del 21 novembre.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
+++ b/GATEWAY/A1#111EBITSRLXXXX/EBITSRL/SUITESTENSA/2.1b34.x/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE Accreditamento\it-fse-accreditamento\GATEWAY\A1#111EBITSRLXXXX\EBITSRL\SUITESTENSA\2.1b34.x\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39303053-0B2B-4C58-8FD8-E7EC851FA51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E817AEC-C95E-40A4-B664-369B644516F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="714">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3538,16 +3538,7 @@
     <t>In questo caso l'evento viene inserito in una coda di uscita gestibile dall'utente tramite una consolle di monitoraggio. Il pdf contiene comunque al suo interno il CDA2 per poi essere conferito al FSE in un secondo momento, grazie al riprocessamento dalla consolle di monitoraggio. La coda è configurabile per avvisare automaticamente il nostro Help Desk</t>
   </si>
   <si>
-    <t>2023-11-22T13:05:21.160Z</t>
-  </si>
-  <si>
-    <t>3c6c3d34d9883680</t>
-  </si>
-  <si>
-    <t>2023-11-22T14:27:11.190Z</t>
-  </si>
-  <si>
-    <t>f8c14d53682dd9aa</t>
+    <t>il campo token JWT "action_id" è valorizzato con un dato fisso "CREATE" e non può essere modificato lato applicativo, ma solo con un untervento forzato e volontario sul motore di integrazione. In produzione non è un caso che può realizzarsi.</t>
   </si>
 </sst>
 </file>
@@ -6473,10 +6464,10 @@
   <dimension ref="A1:T873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="M26" sqref="M26"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6773,7 +6764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -6811,7 +6802,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20">
         <v>8</v>
       </c>
@@ -6849,7 +6840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <v>9</v>
       </c>
@@ -6975,7 +6966,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>13</v>
       </c>
@@ -7013,7 +7004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>14</v>
       </c>
@@ -7051,7 +7042,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>29</v>
       </c>
@@ -7089,7 +7080,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>31</v>
       </c>
@@ -7199,42 +7190,24 @@
       <c r="E21" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="23">
-        <v>45252</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>715</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>716</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>699</v>
-      </c>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="N21" s="25" t="s">
-        <v>703</v>
-      </c>
-      <c r="O21" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="P21" s="35" t="s">
-        <v>608</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>713</v>
+      </c>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="35"/>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
-      <c r="S21" s="37" t="s">
-        <v>702</v>
-      </c>
+      <c r="S21" s="37"/>
       <c r="T21" s="28" t="s">
         <v>68</v>
       </c>
@@ -7255,42 +7228,26 @@
       <c r="E22" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="23">
-        <v>45252</v>
-      </c>
-      <c r="G22" s="24" t="s">
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25" t="s">
+        <v>595</v>
+      </c>
+      <c r="K22" s="25" t="s">
         <v>713</v>
       </c>
-      <c r="H22" s="24" t="s">
-        <v>714</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>699</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="N22" s="25" t="s">
-        <v>703</v>
-      </c>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
       <c r="O22" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="P22" s="35" t="s">
-        <v>608</v>
-      </c>
+      <c r="P22" s="35"/>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
-      <c r="S22" s="37" t="s">
-        <v>702</v>
-      </c>
+      <c r="S22" s="37"/>
       <c r="T22" s="28" t="s">
         <v>68</v>
       </c>
@@ -7487,7 +7444,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>63</v>
       </c>
@@ -7525,7 +7482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>64</v>
       </c>
@@ -7563,7 +7520,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>65</v>
       </c>
@@ -7601,7 +7558,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>66</v>
       </c>
@@ -7639,7 +7596,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20">
         <v>67</v>
       </c>
@@ -7677,7 +7634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
         <v>68</v>
       </c>
@@ -7715,7 +7672,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20">
         <v>69</v>
       </c>
@@ -7753,7 +7710,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="20">
         <v>70</v>
       </c>
@@ -7791,7 +7748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20">
         <v>71</v>
       </c>
@@ -7829,7 +7786,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="20">
         <v>72</v>
       </c>
@@ -7921,7 +7878,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="20">
         <v>74</v>
       </c>
@@ -7959,7 +7916,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20">
         <v>75</v>
       </c>
@@ -7997,7 +7954,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20">
         <v>76</v>
       </c>
@@ -8035,7 +7992,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="20">
         <v>77</v>
       </c>
@@ -8073,7 +8030,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="20">
         <v>78</v>
       </c>
@@ -8111,7 +8068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="20">
         <v>79</v>
       </c>
@@ -8149,7 +8106,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20">
         <v>80</v>
       </c>
@@ -8299,7 +8256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="20">
         <v>83</v>
       </c>
@@ -8393,7 +8350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20">
         <v>85</v>
       </c>
@@ -8431,7 +8388,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="20">
         <v>86</v>
       </c>
@@ -8525,7 +8482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="20">
         <v>88</v>
       </c>
@@ -8563,7 +8520,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20">
         <v>89</v>
       </c>
@@ -8601,7 +8558,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20">
         <v>90</v>
       </c>
@@ -8639,7 +8596,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="20">
         <v>91</v>
       </c>
@@ -8677,7 +8634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="20">
         <v>92</v>
       </c>
@@ -8815,7 +8772,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="20">
         <v>148</v>
       </c>
@@ -8853,7 +8810,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="20">
         <v>149</v>
       </c>
@@ -8891,7 +8848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="20">
         <v>150</v>
       </c>
@@ -8929,7 +8886,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="20">
         <v>151</v>
       </c>
@@ -8967,7 +8924,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="20">
         <v>152</v>
       </c>
@@ -9005,7 +8962,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="20">
         <v>153</v>
       </c>
@@ -9043,7 +9000,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="20">
         <v>154</v>
       </c>
@@ -9081,7 +9038,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="20">
         <v>155</v>
       </c>
@@ -9119,7 +9076,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="20">
         <v>156</v>
       </c>
@@ -9267,7 +9224,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="20">
         <v>159</v>
       </c>
@@ -9305,7 +9262,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="195" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="20">
         <v>160</v>
       </c>
@@ -9359,7 +9316,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="20">
         <v>161</v>
       </c>
@@ -9399,7 +9356,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="20">
         <v>162</v>
       </c>
@@ -9439,7 +9396,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="20">
         <v>163</v>
       </c>
@@ -9479,7 +9436,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="20">
         <v>164</v>
       </c>
@@ -9519,7 +9476,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="20">
         <v>165</v>
       </c>
@@ -9559,7 +9516,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="20">
         <v>166</v>
       </c>
@@ -9599,7 +9556,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="20">
         <v>167</v>
       </c>
@@ -9639,7 +9596,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="20">
         <v>168</v>
       </c>
@@ -9677,7 +9634,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" s="20">
         <v>169</v>
       </c>
@@ -20355,11 +20312,6 @@
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="SI"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>